<commit_message>
histori transaksi di update
</commit_message>
<xml_diff>
--- a/static/template/template.xlsx
+++ b/static/template/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\project\kelontong_mami\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627DF367-80CA-45B2-8BDB-FD4ED6426AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E0F006-5A10-4599-B09A-F80B1F869419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ADC25B1F-B286-458F-9E7B-ACB430C21C31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>barcode</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>6. min_beli_grosir diisikan jumlah minimal pembelian yang akan dianggap sebagai harga grosir</t>
+  </si>
+  <si>
+    <t>harga_beli</t>
+  </si>
+  <si>
+    <t>7. harga_beli diisi dengan harga pembelian (sudah termasuk ppn) untuk penghitungan untung rugi</t>
   </si>
 </sst>
 </file>
@@ -475,21 +481,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786CE997-50A9-4C43-B791-D1D700F2F126}">
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="96.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="96.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -503,16 +510,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -520,8 +530,9 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -529,8 +540,9 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -538,11 +550,12 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="J4" s="3" t="s">
+      <c r="H4" s="1"/>
+      <c r="K4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -550,11 +563,12 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="J5" t="s">
+      <c r="H5" s="1"/>
+      <c r="K5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -562,11 +576,12 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="J6" t="s">
+      <c r="H6" s="1"/>
+      <c r="K6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -574,11 +589,12 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="J7" t="s">
+      <c r="H7" s="1"/>
+      <c r="K7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -586,11 +602,12 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="J8" t="s">
+      <c r="H8" s="1"/>
+      <c r="K8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -598,11 +615,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="J9" t="s">
+      <c r="H9" s="1"/>
+      <c r="K9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -610,11 +628,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="J10" t="s">
+      <c r="H10" s="1"/>
+      <c r="K10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -622,8 +641,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -631,8 +654,9 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -640,8 +664,9 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -649,8 +674,9 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -658,8 +684,9 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -667,8 +694,9 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -676,8 +704,9 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -685,8 +714,9 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -694,8 +724,9 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -703,8 +734,9 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -712,8 +744,9 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -721,8 +754,9 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -730,8 +764,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -739,8 +774,9 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -748,8 +784,9 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -757,8 +794,9 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -766,8 +804,9 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -775,8 +814,9 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -784,8 +824,9 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -793,8 +834,9 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -802,8 +844,9 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -811,8 +854,9 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -820,8 +864,9 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -829,8 +874,9 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -838,8 +884,9 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -847,8 +894,9 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -856,8 +904,9 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -865,8 +914,9 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -874,8 +924,9 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -883,8 +934,9 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -892,8 +944,9 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -901,8 +954,9 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -910,8 +964,9 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -919,8 +974,9 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -928,8 +984,9 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -937,8 +994,9 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -946,8 +1004,9 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -955,8 +1014,9 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -964,8 +1024,9 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -973,8 +1034,9 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -982,8 +1044,9 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -991,8 +1054,9 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1000,8 +1064,9 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1009,8 +1074,9 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1018,8 +1084,9 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1027,8 +1094,9 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1036,8 +1104,9 @@
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1045,8 +1114,9 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1054,8 +1124,9 @@
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1063,8 +1134,9 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1072,8 +1144,9 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1081,8 +1154,9 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1090,8 +1164,9 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1099,8 +1174,9 @@
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1108,8 +1184,9 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1117,8 +1194,9 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1126,8 +1204,9 @@
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1135,8 +1214,9 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1144,8 +1224,9 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1153,8 +1234,9 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1162,8 +1244,9 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1171,8 +1254,9 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1180,8 +1264,9 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1189,8 +1274,9 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1198,8 +1284,9 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1207,8 +1294,9 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1216,8 +1304,9 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1225,8 +1314,9 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1234,8 +1324,9 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1243,8 +1334,9 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1252,8 +1344,9 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1261,8 +1354,9 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="1"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1270,8 +1364,9 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1279,8 +1374,9 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1288,8 +1384,9 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1297,8 +1394,9 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1306,8 +1404,9 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1315,8 +1414,9 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1324,8 +1424,9 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1333,8 +1434,9 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1342,8 +1444,9 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1351,8 +1454,9 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="1"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1360,8 +1464,9 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1369,8 +1474,9 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1378,8 +1484,9 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="1"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1387,8 +1494,9 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="1"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1396,8 +1504,9 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="1"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1405,8 +1514,9 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="1"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1414,8 +1524,9 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="1"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1423,8 +1534,9 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="1"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1432,8 +1544,9 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="1"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1441,8 +1554,9 @@
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="1"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1450,8 +1564,9 @@
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103" s="1"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1459,8 +1574,9 @@
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104" s="1"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1468,8 +1584,9 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105" s="1"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1477,8 +1594,9 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="1"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1486,8 +1604,9 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="1"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1495,8 +1614,9 @@
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="1"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1504,8 +1624,9 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="1"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1513,8 +1634,9 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="1"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1522,8 +1644,9 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="1"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1531,8 +1654,9 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H112" s="1"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -1540,8 +1664,9 @@
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H113" s="1"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -1549,8 +1674,9 @@
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H114" s="1"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1558,8 +1684,9 @@
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H115" s="1"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -1567,8 +1694,9 @@
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116" s="1"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -1576,8 +1704,9 @@
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H117" s="1"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -1585,8 +1714,9 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H118" s="1"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -1594,8 +1724,9 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H119" s="1"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -1603,8 +1734,9 @@
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H120" s="1"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -1612,8 +1744,9 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H121" s="1"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -1621,8 +1754,9 @@
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H122" s="1"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -1630,8 +1764,9 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H123" s="1"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -1639,8 +1774,9 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H124" s="1"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -1648,8 +1784,9 @@
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H125" s="1"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -1657,8 +1794,9 @@
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -1666,8 +1804,9 @@
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H127" s="1"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -1675,8 +1814,9 @@
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H128" s="1"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -1684,8 +1824,9 @@
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H129" s="1"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -1693,8 +1834,9 @@
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H130" s="1"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -1702,8 +1844,9 @@
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H131" s="1"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -1711,8 +1854,9 @@
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H132" s="1"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -1720,8 +1864,9 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H133" s="1"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -1729,6 +1874,7 @@
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
keterangan ditambahkan di upload download barang, user aktif atau tidak
</commit_message>
<xml_diff>
--- a/static/template/template.xlsx
+++ b/static/template/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\project\kelontong_mami\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E0F006-5A10-4599-B09A-F80B1F869419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F42E90-A0BD-4D9E-B853-138F319C7624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ADC25B1F-B286-458F-9E7B-ACB430C21C31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>barcode</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>7. harga_beli diisi dengan harga pembelian (sudah termasuk ppn) untuk penghitungan untung rugi</t>
+  </si>
+  <si>
+    <t>keterangan</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786CE997-50A9-4C43-B791-D1D700F2F126}">
-  <dimension ref="A1:K134"/>
+  <dimension ref="A1:L134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +496,11 @@
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="96.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="96.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -521,8 +525,11 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -531,8 +538,9 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -541,8 +549,9 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -551,11 +560,12 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="K4" s="3" t="s">
+      <c r="I4" s="1"/>
+      <c r="L4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -564,11 +574,12 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="K5" t="s">
+      <c r="I5" s="1"/>
+      <c r="L5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -577,11 +588,12 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="K6" t="s">
+      <c r="I6" s="1"/>
+      <c r="L6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -590,11 +602,12 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="K7" t="s">
+      <c r="I7" s="1"/>
+      <c r="L7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -603,11 +616,12 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="K8" t="s">
+      <c r="I8" s="1"/>
+      <c r="L8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -616,11 +630,12 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="K9" t="s">
+      <c r="I9" s="1"/>
+      <c r="L9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -629,11 +644,12 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="K10" t="s">
+      <c r="I10" s="1"/>
+      <c r="L10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -642,11 +658,12 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="K11" t="s">
+      <c r="I11" s="1"/>
+      <c r="L11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -655,8 +672,9 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -665,8 +683,9 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -675,8 +694,9 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -685,8 +705,9 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -695,8 +716,9 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -705,8 +727,9 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -715,8 +738,9 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -725,8 +749,9 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -735,8 +760,9 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -745,8 +771,9 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -755,8 +782,9 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -765,8 +793,9 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -775,8 +804,9 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -785,8 +815,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -795,8 +826,9 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -805,8 +837,9 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -815,8 +848,9 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -825,8 +859,9 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -835,8 +870,9 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -845,8 +881,9 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -855,8 +892,9 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -865,8 +903,9 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -875,8 +914,9 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -885,8 +925,9 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -895,8 +936,9 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -905,8 +947,9 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -915,8 +958,9 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -925,8 +969,9 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -935,8 +980,9 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -945,8 +991,9 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -955,8 +1002,9 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -965,8 +1013,9 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -975,8 +1024,9 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -985,8 +1035,9 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -995,8 +1046,9 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1005,8 +1057,9 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1015,8 +1068,9 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1025,8 +1079,9 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1035,8 +1090,9 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1045,8 +1101,9 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1055,8 +1112,9 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1065,8 +1123,9 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1075,8 +1134,9 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1085,8 +1145,9 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1095,8 +1156,9 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1105,8 +1167,9 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1115,8 +1178,9 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1125,8 +1189,9 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1135,8 +1200,9 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1145,8 +1211,9 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1155,8 +1222,9 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1165,8 +1233,9 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1175,8 +1244,9 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1185,8 +1255,9 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1195,8 +1266,9 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1205,8 +1277,9 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1215,8 +1288,9 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1225,8 +1299,9 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1235,8 +1310,9 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1245,8 +1321,9 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1255,8 +1332,9 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1265,8 +1343,9 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1275,8 +1354,9 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1285,8 +1365,9 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1295,8 +1376,9 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1305,8 +1387,9 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1315,8 +1398,9 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1325,8 +1409,9 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1335,8 +1420,9 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1345,8 +1431,9 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1355,8 +1442,9 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1365,8 +1453,9 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1375,8 +1464,9 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1385,8 +1475,9 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1395,8 +1486,9 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1405,8 +1497,9 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1415,8 +1508,9 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1425,8 +1519,9 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1435,8 +1530,9 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1445,8 +1541,9 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1455,8 +1552,9 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1465,8 +1563,9 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1475,8 +1574,9 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1485,8 +1585,9 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1495,8 +1596,9 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1505,8 +1607,9 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1515,8 +1618,9 @@
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1525,8 +1629,9 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1535,8 +1640,9 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1545,8 +1651,9 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1555,8 +1662,9 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1565,8 +1673,9 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1575,8 +1684,9 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1585,8 +1695,9 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="1"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1595,8 +1706,9 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1605,8 +1717,9 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="1"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1615,8 +1728,9 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1625,8 +1739,9 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1635,8 +1750,9 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="1"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1645,8 +1761,9 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="1"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1655,8 +1772,9 @@
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="1"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -1665,8 +1783,9 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="1"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -1675,8 +1794,9 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1685,8 +1805,9 @@
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="1"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -1695,8 +1816,9 @@
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="1"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -1705,8 +1827,9 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="1"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -1715,8 +1838,9 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -1725,8 +1849,9 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -1735,8 +1860,9 @@
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -1745,8 +1871,9 @@
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -1755,8 +1882,9 @@
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -1765,8 +1893,9 @@
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="1"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -1775,8 +1904,9 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="1"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -1785,8 +1915,9 @@
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="1"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -1795,8 +1926,9 @@
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -1805,8 +1937,9 @@
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -1815,8 +1948,9 @@
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="1"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -1825,8 +1959,9 @@
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="1"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -1835,8 +1970,9 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="1"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -1845,8 +1981,9 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -1855,8 +1992,9 @@
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -1865,8 +2003,9 @@
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -1875,6 +2014,7 @@
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
penambahan keterangan untuk template_posmi.xlsx
</commit_message>
<xml_diff>
--- a/static/template/template.xlsx
+++ b/static/template/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\project\kelontong_mami\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F42E90-A0BD-4D9E-B853-138F319C7624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C674A0-CFD1-4C24-94E5-A86B7F994E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ADC25B1F-B286-458F-9E7B-ACB430C21C31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>barcode</t>
   </si>
@@ -87,6 +87,48 @@
   </si>
   <si>
     <t>keterangan</t>
+  </si>
+  <si>
+    <t>Catatan tambahan:</t>
+  </si>
+  <si>
+    <t>1. Semua Kolom harus diisi kecuali kolom keterangan</t>
+  </si>
+  <si>
+    <t>2. apabila barang tidak memiliki barcode bisa diisi dengan angka atau huruf dan harus unik, misalnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    dibuat kode aa1 atau aa2 atau aa3 atau 123 atau 124 dan lain-lain</t>
+  </si>
+  <si>
+    <t>3. apabila harga penjualan tidak ada mode grosir, min_beli_grosir diisi angka 1</t>
+  </si>
+  <si>
+    <t>Barang Contoh</t>
+  </si>
+  <si>
+    <t>PCS</t>
+  </si>
+  <si>
+    <t>barang tanpa grosir</t>
+  </si>
+  <si>
+    <t>Barang Contoh 2</t>
+  </si>
+  <si>
+    <t>PACK</t>
+  </si>
+  <si>
+    <t>barang grosir dengan minimal pembelian 2</t>
+  </si>
+  <si>
+    <t>abc1</t>
+  </si>
+  <si>
+    <t>Barang Contoh 3</t>
+  </si>
+  <si>
+    <t>barang dengan kode huruf</t>
   </si>
 </sst>
 </file>
@@ -486,17 +528,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786CE997-50A9-4C43-B791-D1D700F2F126}">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="40" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="96.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -530,37 +573,91 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="A2" s="1">
+        <v>123</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>200000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>230000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>230000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="1">
+        <v>124</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>120000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>140000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>135000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F4" s="1">
+        <v>28000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>25000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="L4" s="3" t="s">
         <v>7</v>
       </c>
@@ -695,6 +792,9 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -706,6 +806,9 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
+      <c r="L15" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -717,8 +820,11 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -728,8 +834,11 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -739,8 +848,11 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -751,7 +863,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -762,7 +874,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -773,7 +885,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -784,7 +896,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -795,7 +907,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -806,7 +918,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -817,7 +929,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -828,7 +940,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -839,7 +951,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -850,7 +962,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -861,7 +973,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -872,7 +984,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -883,7 +995,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>

</xml_diff>

<commit_message>
menambahkan tombol hapus di samping barang untuk hapus
</commit_message>
<xml_diff>
--- a/static/template/template.xlsx
+++ b/static/template/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\project\kelontong_mami\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C674A0-CFD1-4C24-94E5-A86B7F994E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D969022-0586-4897-BBD4-FBE866322ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ADC25B1F-B286-458F-9E7B-ACB430C21C31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>barcode</t>
   </si>
@@ -95,12 +95,6 @@
     <t>1. Semua Kolom harus diisi kecuali kolom keterangan</t>
   </si>
   <si>
-    <t>2. apabila barang tidak memiliki barcode bisa diisi dengan angka atau huruf dan harus unik, misalnya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    dibuat kode aa1 atau aa2 atau aa3 atau 123 atau 124 dan lain-lain</t>
-  </si>
-  <si>
     <t>3. apabila harga penjualan tidak ada mode grosir, min_beli_grosir diisi angka 1</t>
   </si>
   <si>
@@ -122,13 +116,10 @@
     <t>barang grosir dengan minimal pembelian 2</t>
   </si>
   <si>
-    <t>abc1</t>
-  </si>
-  <si>
-    <t>Barang Contoh 3</t>
-  </si>
-  <si>
-    <t>barang dengan kode huruf</t>
+    <t>2. apabila barang tidak memiliki barcode bisa diisi dengan angka dan harus unik, misalnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    dibuat kode 120 atau 121 atau 122 atau 12334 atau 12434 dan lain-lain</t>
   </si>
 </sst>
 </file>
@@ -528,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786CE997-50A9-4C43-B791-D1D700F2F126}">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,10 +568,10 @@
         <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -598,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -606,10 +597,10 @@
         <v>124</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -627,37 +618,19 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>20000</v>
-      </c>
-      <c r="F4" s="1">
-        <v>28000</v>
-      </c>
-      <c r="G4" s="1">
-        <v>25000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="L4" s="3" t="s">
         <v>7</v>
       </c>
@@ -821,7 +794,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="L16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -835,7 +808,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="L17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -849,7 +822,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="L18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>